<commit_message>
All in one class json file added
</commit_message>
<xml_diff>
--- a/unpackers/input/input.xlsx
+++ b/unpackers/input/input.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danylopiatyhorets/Desktop/Hackathon/unpackers/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D7DDF4-B6A2-2A4C-B2EF-5023859A4E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82427CEE-E9E3-2B43-8867-44D28DA96AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14000" xr2:uid="{19D55572-F2FA-174A-8658-4B24A432AF65}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{19D55572-F2FA-174A-8658-4B24A432AF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Sarah Adams</t>
-  </si>
-  <si>
-    <t>Michael Brown</t>
-  </si>
-  <si>
     <t>Heartrate</t>
   </si>
   <si>
@@ -67,13 +62,67 @@
     <t>5.5 hours</t>
   </si>
   <si>
-    <t>120/80 mmHg</t>
-  </si>
-  <si>
     <t>130/75 mmHg</t>
   </si>
   <si>
     <t>BloodPressure</t>
+  </si>
+  <si>
+    <t>125/80 mmHg</t>
+  </si>
+  <si>
+    <t>Sophia Wilson</t>
+  </si>
+  <si>
+    <t>Liam Brown</t>
+  </si>
+  <si>
+    <t>Olivia Taylor</t>
+  </si>
+  <si>
+    <t>Noah Davis</t>
+  </si>
+  <si>
+    <t>Ella Brown</t>
+  </si>
+  <si>
+    <t>Charlotte Anderson</t>
+  </si>
+  <si>
+    <t>140/85 mmHg</t>
+  </si>
+  <si>
+    <t>70/45 mmHg</t>
+  </si>
+  <si>
+    <t>90/60 mmHg</t>
+  </si>
+  <si>
+    <t>135/75 mmHg</t>
+  </si>
+  <si>
+    <t>62 bpm</t>
+  </si>
+  <si>
+    <t>122 bpm</t>
+  </si>
+  <si>
+    <t>67 bpm</t>
+  </si>
+  <si>
+    <t>87 bpm</t>
+  </si>
+  <si>
+    <t>7.5 hours</t>
+  </si>
+  <si>
+    <t>9 hours</t>
+  </si>
+  <si>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>8 hours</t>
   </si>
 </sst>
 </file>
@@ -97,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,13 +154,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,15 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAF2E61-6AF0-0F4D-BB43-433B29BC6E11}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -443,51 +505,122 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>45241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>45239</v>
       </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>